<commit_message>
Fixed AWS recommendations in the CFN template for WHD
</commit_message>
<xml_diff>
--- a/aws/whd/ProductForm/AmazonAMI-WHD-12_5_0_1257.xlsx
+++ b/aws/whd/ProductForm/AmazonAMI-WHD-12_5_0_1257.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madhuvj\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\marketplaces\aws\whd\ProductForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1248,9 +1248,6 @@
 </t>
   </si>
   <si>
-    <t>ami-a00636b7</t>
-  </si>
-  <si>
     <t>https://support.solarwinds.com/Success_Center/Web_Help_Desk_(WHD)/WHD_Admin_Guide</t>
   </si>
   <si>
@@ -1261,6 +1258,9 @@
   </si>
   <si>
     <t>SolarWinds_WHD_12.5</t>
+  </si>
+  <si>
+    <t>ami-24f3f033</t>
   </si>
 </sst>
 </file>
@@ -5279,10 +5279,10 @@
   </sheetPr>
   <dimension ref="A1:GM1180"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AB1" sqref="AB1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="15.9" customHeight="1"/>
@@ -5925,13 +5925,13 @@
     </row>
     <row r="2" spans="1:195" s="91" customFormat="1" ht="317.39999999999998">
       <c r="A2" s="93" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2" s="82" t="s">
         <v>332</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D2" s="83" t="s">
         <v>341</v>
@@ -6002,7 +6002,7 @@
       <c r="Z2" s="90"/>
       <c r="AA2" s="90"/>
       <c r="AB2" s="107" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="AC2" s="97"/>
       <c r="AD2" s="94" t="s">
@@ -6313,10 +6313,10 @@
         <v>376</v>
       </c>
       <c r="GL2" s="112" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="GM2" s="112" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="3" spans="1:195" s="32" customFormat="1" ht="14.4">
@@ -67159,18 +67159,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67288,6 +67288,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B5DC2E0-0871-44B1-89B4-ACA1409A331A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{926ACF4F-A83A-4655-A95E-1B7425DC877E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -67298,14 +67306,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B5DC2E0-0871-44B1-89B4-ACA1409A331A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>